<commit_message>
modified:   gwas_atacseq_overlap/gregor/merge_peaks.R 	modified:   gwas_atacseq_overlap/gregor/overlap_enrichment.R 	modified:   gwas_atacseq_overlap/papers/GREGOR_SuppTable1.xlsx 	modified:   hcasmc_specific_open_chromatin/mds_open_chromatin_merged_peaks.R 	modified:   pipe.sh
</commit_message>
<xml_diff>
--- a/gwas_atacseq_overlap/papers/GREGOR_SuppTable1.xlsx
+++ b/gwas_atacseq_overlap/papers/GREGOR_SuppTable1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="S1_DHS_Tissue_Groups" sheetId="6" r:id="rId1"/>
@@ -1486,7 +1486,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1633,6 +1633,22 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2030,7 +2046,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2073,6 +2089,20 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2099,7 +2129,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="56">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2128,11 +2158,25 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2442,9 +2486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>